<commit_message>
Update Finanzuebersicht and delete it from Old_Finanzentwicklung
</commit_message>
<xml_diff>
--- a/Old_Finanzentwicklung_HelloBank_FFB.xlsx
+++ b/Old_Finanzentwicklung_HelloBank_FFB.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cpreissl/Documents/Finance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF53C21-98E2-1C41-BA03-E4E5F8C546D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6159E37-E7CE-714F-BFA1-0169569BBE86}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="45100" windowHeight="21900" activeTab="2" xr2:uid="{97D30251-3E24-4479-8B6A-67D42D9B0E9A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="45100" windowHeight="21900" activeTab="1" xr2:uid="{97D30251-3E24-4479-8B6A-67D42D9B0E9A}"/>
   </bookViews>
   <sheets>
     <sheet name="FFB Entwicklung" sheetId="1" r:id="rId1"/>
     <sheet name="FFB Zusammensetzung" sheetId="2" r:id="rId2"/>
-    <sheet name="Strategie" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Jänner</t>
   </si>
@@ -149,81 +148,16 @@
   </si>
   <si>
     <t>aktueller Stand 27.1.2021</t>
-  </si>
-  <si>
-    <t>ING</t>
-  </si>
-  <si>
-    <t>Sparkasse</t>
-  </si>
-  <si>
-    <t>FFB</t>
-  </si>
-  <si>
-    <t>Bar zuhause</t>
-  </si>
-  <si>
-    <t>Paypal</t>
-  </si>
-  <si>
-    <t>Gesamt</t>
-  </si>
-  <si>
-    <t>Gesamt in Cash</t>
-  </si>
-  <si>
-    <t>Gesamt in Wertpapiere</t>
-  </si>
-  <si>
-    <t>Etrade (Apple)</t>
-  </si>
-  <si>
-    <t>Ziel</t>
-  </si>
-  <si>
-    <t>ToDo</t>
-  </si>
-  <si>
-    <t>MSCI World Small Cap Index</t>
-  </si>
-  <si>
-    <t>MSCI ACWI (inkl. NASDAQ100, S&amp;P500, MSCI World)</t>
-  </si>
-  <si>
-    <t>Von Cash zu Wertpapier (nach Flatex)</t>
-  </si>
-  <si>
-    <t>Flatex Depot</t>
-  </si>
-  <si>
-    <t>Flatex Cashkonto</t>
-  </si>
-  <si>
-    <t>In Flatex Depot Aktien-Verteilung Regime Normal nach Dr. Beck:</t>
-  </si>
-  <si>
-    <t>Situation am 17.03.2021</t>
-  </si>
-  <si>
-    <t>Cash-Quote von</t>
-  </si>
-  <si>
-    <t>Wertpapier-Quote von</t>
-  </si>
-  <si>
-    <t>Führt zu einem Depotbestand bei Flatex</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;€&quot;\ #,##0.00"/>
-    <numFmt numFmtId="165" formatCode="#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]"/>
-    <numFmt numFmtId="166" formatCode="#,##0.00\ [$€-1];[Red]\-#,##0.00\ [$€-1]"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -291,23 +225,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -324,18 +243,8 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -343,30 +252,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -378,24 +270,10 @@
     <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="7" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="8" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="4" borderId="1" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="10" fillId="5" borderId="1" xfId="4" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="10" fillId="5" borderId="1" xfId="4" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="9" fillId="4" borderId="1" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="10" fillId="5" borderId="1" xfId="4" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Calculation" xfId="4" builtinId="22"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Input" xfId="3" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1207,7 +1085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AD1EBB5-758E-4082-8ACC-069A8489DF27}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -1377,223 +1255,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D74A1D7F-7BD7-4C7A-B226-A53EC8FD1471}">
-  <dimension ref="A1:I13"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:G7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="20.83203125" customWidth="1"/>
-    <col min="6" max="6" width="24.83203125" customWidth="1"/>
-    <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="F1" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-    </row>
-    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="13">
-        <v>58525</v>
-      </c>
-      <c r="F2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G2" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="H2" s="14">
-        <f>G4*G2</f>
-        <v>59400.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="13">
-        <v>3042</v>
-      </c>
-      <c r="F3" t="s">
-        <v>57</v>
-      </c>
-      <c r="G3" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="H3" s="14">
-        <f>G4*G3</f>
-        <v>59400.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="13">
-        <v>22580</v>
-      </c>
-      <c r="F4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4" s="14">
-        <f>B13</f>
-        <v>118801</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5" s="13">
-        <v>17530</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="13">
-        <v>11090</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-    </row>
-    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="13">
-        <v>4900</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="14">
-        <f>B11-H2</f>
-        <v>18770.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="13">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="13">
-        <v>520</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-    </row>
-    <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="F10" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="H10" s="16">
-        <f>1-H11</f>
-        <v>0.875</v>
-      </c>
-      <c r="I10" s="18">
-        <f>H13*H10</f>
-        <v>31762.9375</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="14">
-        <f>B2+B7+B8+B3+B6</f>
-        <v>78171</v>
-      </c>
-      <c r="C11" s="15">
-        <f>B11/B13</f>
-        <v>0.65799951178862126</v>
-      </c>
-      <c r="F11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H11" s="16">
-        <v>0.125</v>
-      </c>
-      <c r="I11" s="18">
-        <f>H13*H11</f>
-        <v>4537.5625</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="14">
-        <f>B4+B5+B9</f>
-        <v>40630</v>
-      </c>
-      <c r="C12" s="15">
-        <f>B12/B13</f>
-        <v>0.34200048821137868</v>
-      </c>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="14">
-        <f>SUM(B2:B9)</f>
-        <v>118801</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="G13" s="11"/>
-      <c r="H13" s="14">
-        <f>H7+B5</f>
-        <v>36300.5</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F9:I9"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>